<commit_message>
Working UI ( changing panels )
Created a default character in the Character Manager, Updates correctly
when pressing 'C' and opens the panel + edited planning
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Time Spent</t>
   </si>
@@ -81,13 +81,16 @@
   </si>
   <si>
     <t>End game condition ( win/lose )</t>
+  </si>
+  <si>
+    <t>Creating Unity UI with default Character ( test )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,8 +98,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,7 +128,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,12 +163,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -454,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,13 +506,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -482,10 +520,10 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <v>6.25E-2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -493,99 +531,111 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 3 test characters + HUD
HUD no works ( simple ), still some stuff I could add ( armor type,
class, ... )
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Time Spent</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Creating Unity UI with default Character ( test )</t>
+  </si>
+  <si>
+    <t>Spawn 3 test characters</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Did it in parts, most of the structure stuff is done</t>
   </si>
 </sst>
 </file>
@@ -107,7 +116,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +156,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -178,6 +199,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -492,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,9 +528,11 @@
     <col min="1" max="1" width="87" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -515,8 +542,11 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -527,15 +557,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -546,15 +582,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -562,75 +598,86 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited UI + Character creation works
Created character via game manager and UI updates correctly, next step
is to spawn them in the level using the Visua Character
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Time Spent</t>
   </si>
@@ -53,9 +53,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>Writing character</t>
-  </si>
-  <si>
     <t>Spawn 3 characters</t>
   </si>
   <si>
@@ -93,6 +90,18 @@
   </si>
   <si>
     <t>Did it in parts, most of the structure stuff is done</t>
+  </si>
+  <si>
+    <t>Let characters follow selected character ( no clipping -&gt; navmesh )</t>
+  </si>
+  <si>
+    <t>Let enemies track ( follow ) selected character ( no clipping -&gt; navmesh ). When close enough, attack closest of 3 characters</t>
+  </si>
+  <si>
+    <t>Writing character ( = visualize the prefab and spawn it in level with correct stats )</t>
+  </si>
+  <si>
+    <t>UIManager not entirely clear, UI seems to work without it</t>
   </si>
 </sst>
 </file>
@@ -517,15 +526,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87" customWidth="1"/>
+    <col min="1" max="1" width="111.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="60.42578125" customWidth="1"/>
@@ -543,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -568,12 +577,12 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>2.7777777777777776E-2</v>
@@ -589,10 +598,13 @@
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -600,7 +612,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>1.3888888888888888E-2</v>
@@ -611,15 +623,18 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>8</v>
@@ -627,7 +642,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
@@ -635,7 +650,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -643,23 +658,29 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>8</v>
@@ -667,17 +688,36 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added win/lose and logic to UI ( health system )
Attack and defense now factor in damage done by character / enemy
Game can end ( check if there are still enemies to be killed of if all 3
characters are dead ) -> game pauzes
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Time Spent</t>
   </si>
@@ -92,12 +92,6 @@
     <t>Did it in parts, most of the structure stuff is done</t>
   </si>
   <si>
-    <t>Let characters follow selected character ( no clipping -&gt; navmesh )</t>
-  </si>
-  <si>
-    <t>Let enemies track ( follow ) selected character ( no clipping -&gt; navmesh ). When close enough, attack closest of 3 characters</t>
-  </si>
-  <si>
     <t>Writing character ( = visualize the prefab and spawn it in level with correct stats )</t>
   </si>
   <si>
@@ -110,7 +104,25 @@
     <t>No direct link between UI and logic yet, but can easily add it, not necessary yet</t>
   </si>
   <si>
-    <t>HOLD</t>
+    <t>Character manager</t>
+  </si>
+  <si>
+    <t>UI Manager</t>
+  </si>
+  <si>
+    <t>I did it in parts and added some small methods later on ( because of how I made the enemies etc. )</t>
+  </si>
+  <si>
+    <t>Let enemies track ( follow ) selected character ( navmesh ). When close enough, attack closest of 3 characters</t>
+  </si>
+  <si>
+    <t>Let characters follow selected character ( navmesh )</t>
+  </si>
+  <si>
+    <t>Now enemy tracks always selected character, I need a check to see if one of the enemies is close enough</t>
+  </si>
+  <si>
+    <t>Cleanup code</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,12 +179,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -191,7 +197,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF5757"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,7 +218,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -222,12 +227,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -547,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,21 +566,21 @@
     <col min="1" max="1" width="111.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="72.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="94.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -616,33 +624,36 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="1">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
       <c r="B7" s="1">
-        <v>1.3888888888888888E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
@@ -650,21 +661,24 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
-        <v>3.125E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -672,26 +686,32 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>1.3888888888888888E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
@@ -699,10 +719,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>7.6388888888888895E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
@@ -710,18 +730,21 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>2.0833333333333332E-2</v>
+        <v>7.6388888888888895E-2</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
@@ -729,36 +752,78 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
       <c r="B18" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Redid end game + added inventory panel
Found more elegant solution to the end game calculations
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Time Spent</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>Cleanup code</t>
+  </si>
+  <si>
+    <t>Revisit end game, more elegant solution</t>
+  </si>
+  <si>
+    <t>This cost me a lot of time due to testing</t>
+  </si>
+  <si>
+    <t>Inventory ( panel )</t>
+  </si>
+  <si>
+    <t>Seperated character panel and inventory panel ( put actual items on the inventory panel )</t>
   </si>
 </sst>
 </file>
@@ -555,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,9 +833,37 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleaned up some code, fixed some small bugs
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Time Spent</t>
   </si>
@@ -113,9 +113,6 @@
     <t>I did it in parts and added some small methods later on ( because of how I made the enemies etc. )</t>
   </si>
   <si>
-    <t>Let enemies track ( follow ) selected character ( navmesh ). When close enough, attack closest of 3 characters</t>
-  </si>
-  <si>
     <t>Let characters follow selected character ( navmesh )</t>
   </si>
   <si>
@@ -135,6 +132,12 @@
   </si>
   <si>
     <t>Seperated character panel and inventory panel ( put actual items on the inventory panel )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let enemies track ( follow ) selected character ( navmesh ). </t>
+  </si>
+  <si>
+    <t>When close enough, attack closest of 3 characters</t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +800,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1">
         <v>4.1666666666666664E-2</v>
@@ -819,52 +822,61 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>6</v>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="1">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1">
-        <v>6.9444444444444441E-3</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>8</v>
+        <v>34</v>
+      </c>
+      <c r="B24" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleanud up code, fixed some bugs
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Time Spent</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>When close enough, attack closest of 3 characters</t>
+  </si>
+  <si>
+    <t>I'll keep on cleaning until deadline</t>
   </si>
 </sst>
 </file>
@@ -206,13 +209,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFB7C624"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,10 +249,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -259,6 +262,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB7C624"/>
+      <color rgb="FF58B000"/>
       <color rgb="FFFF5757"/>
     </mruColors>
   </colors>
@@ -573,7 +578,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +655,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="1">
@@ -664,7 +669,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1">
@@ -839,7 +844,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -875,8 +880,14 @@
       <c r="A25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition to enemy following behaviour
when enemy is close enough to a character, persue this one instead of
selected character
improved UI and weapon behaviour
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Time Spent</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Writing managers ( game, character, UI )</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>Spawn 3 characters</t>
@@ -170,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,12 +212,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB7C624"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -238,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -259,7 +250,6 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -584,7 +574,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,12 +622,12 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>2.7777777777777776E-2</v>
@@ -657,12 +647,12 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1">
         <v>0.125</v>
@@ -671,12 +661,12 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>1.0416666666666666E-2</v>
@@ -687,7 +677,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>0.10416666666666667</v>
@@ -696,12 +686,12 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>1.3888888888888888E-2</v>
@@ -712,7 +702,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>4.1666666666666664E-2</v>
@@ -723,7 +713,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>3.125E-2</v>
@@ -734,7 +724,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>8.3333333333333329E-2</v>
@@ -745,7 +735,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>3.125E-2</v>
@@ -756,7 +746,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>1.3888888888888888E-2</v>
@@ -767,7 +757,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <v>7.6388888888888895E-2</v>
@@ -776,12 +766,12 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>7.6388888888888895E-2</v>
@@ -792,7 +782,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>0.10416666666666667</v>
@@ -803,7 +793,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>2.0833333333333332E-2</v>
@@ -814,7 +804,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>1.3888888888888888E-2</v>
@@ -825,7 +815,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1">
         <v>4.1666666666666664E-2</v>
@@ -836,7 +826,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>6.9444444444444441E-3</v>
@@ -847,7 +837,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1">
         <v>8.3333333333333329E-2</v>
@@ -856,21 +846,23 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="9" t="s">
-        <v>8</v>
+        <v>36</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>6.25E-2</v>
@@ -879,12 +871,12 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="1">
         <v>6.9444444444444441E-3</v>
@@ -893,21 +885,21 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added menu, updated ranger and warrior
Almost done, some code cleanup to do
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>Time Spent</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Sword only works within range of enemy, Ranger shoots his arrows, Wizard can only heal</t>
+  </si>
+  <si>
+    <t>Added menu screen with info</t>
   </si>
 </sst>
 </file>
@@ -571,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,15 +893,26 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B27" s="1">
         <v>0</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleaned up code for deadline
Set healer attack stat to 0 ( can't attack anyway )
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Time Spent</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Writing structure in scripts ( members and functions )</t>
-  </si>
-  <si>
-    <t>BUSY</t>
   </si>
   <si>
     <t>Writing managers ( game, character, UI )</t>
@@ -170,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,12 +210,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB7C624"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -232,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -252,7 +243,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -577,7 +567,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,12 +615,12 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>2.7777777777777776E-2</v>
@@ -641,7 +631,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>0.13541666666666666</v>
@@ -650,12 +640,12 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>0.125</v>
@@ -664,12 +654,12 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>1.0416666666666666E-2</v>
@@ -680,7 +670,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>0.10416666666666667</v>
@@ -689,12 +679,12 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>1.3888888888888888E-2</v>
@@ -705,7 +695,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
         <v>4.1666666666666664E-2</v>
@@ -716,7 +706,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>3.125E-2</v>
@@ -727,7 +717,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>8.3333333333333329E-2</v>
@@ -738,7 +728,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1">
         <v>3.125E-2</v>
@@ -749,7 +739,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1">
         <v>1.3888888888888888E-2</v>
@@ -760,7 +750,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1">
         <v>7.6388888888888895E-2</v>
@@ -769,12 +759,12 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1">
         <v>7.6388888888888895E-2</v>
@@ -785,7 +775,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1">
         <v>0.10416666666666667</v>
@@ -796,7 +786,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1">
         <v>2.0833333333333332E-2</v>
@@ -807,7 +797,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
         <v>1.3888888888888888E-2</v>
@@ -818,7 +808,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1">
         <v>4.1666666666666664E-2</v>
@@ -829,7 +819,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
         <v>6.9444444444444441E-3</v>
@@ -840,7 +830,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1">
         <v>8.3333333333333329E-2</v>
@@ -849,12 +839,12 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1">
         <v>1.7361111111111112E-2</v>
@@ -865,7 +855,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1">
         <v>6.25E-2</v>
@@ -874,12 +864,12 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1">
         <v>6.9444444444444441E-3</v>
@@ -888,12 +878,12 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1">
         <v>1.3888888888888888E-2</v>
@@ -904,16 +894,16 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>6</v>
+      <c r="C27" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>